<commit_message>
new Trapping rain water added
</commit_message>
<xml_diff>
--- a/NeetCode_150_FAANG_Tracker.xlsx
+++ b/NeetCode_150_FAANG_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faizan/faizan/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86AB43F-436D-1348-86BE-46A3C1DB1EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCFF84E-5B4F-2E41-B34C-89CCC59A0425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="135">
   <si>
     <t>Order</t>
   </si>
@@ -390,6 +390,42 @@
   </si>
   <si>
     <t>day7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 🟡</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> main logic here is length-prefixed serialization</t>
+  </si>
+  <si>
+    <t>day8</t>
+  </si>
+  <si>
+    <t>do it later</t>
+  </si>
+  <si>
+    <t>day 9</t>
+  </si>
+  <si>
+    <t>done only important logic is regex and ascii to convert it/[a-z0-9]/i.test(s[r])</t>
+  </si>
+  <si>
+    <t>day9</t>
+  </si>
+  <si>
+    <t>solve self by bruteForce but now go for optimal</t>
+  </si>
+  <si>
+    <t>✅ 🟡</t>
+  </si>
+  <si>
+    <t>✅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solve by slef because two pointer clear </t>
+  </si>
+  <si>
+    <t>day10</t>
   </si>
 </sst>
 </file>
@@ -738,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -748,7 +784,7 @@
     <col min="4" max="4" width="17.1640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="7" max="7" width="18.1640625" customWidth="1"/>
-    <col min="8" max="8" width="44.5" customWidth="1"/>
+    <col min="8" max="8" width="49.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -852,7 +888,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>46009</v>
       </c>
@@ -930,9 +966,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>46186</v>
+        <v>46035</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -949,8 +985,17 @@
       <c r="F8" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>46036</v>
+      </c>
       <c r="B9">
         <v>8</v>
       </c>
@@ -963,8 +1008,20 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>46036</v>
+      </c>
       <c r="B10">
         <v>9</v>
       </c>
@@ -977,8 +1034,20 @@
       <c r="E10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G10" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>46037</v>
+      </c>
       <c r="B11">
         <v>10</v>
       </c>
@@ -991,8 +1060,20 @@
       <c r="E11" t="s">
         <v>8</v>
       </c>
+      <c r="F11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>46037</v>
+      </c>
       <c r="B12">
         <v>11</v>
       </c>
@@ -1005,8 +1086,17 @@
       <c r="E12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>46047</v>
+      </c>
       <c r="B13">
         <v>12</v>
       </c>
@@ -1019,8 +1109,20 @@
       <c r="E13" t="s">
         <v>20</v>
       </c>
+      <c r="F13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>46047</v>
+      </c>
       <c r="B14">
         <v>13</v>
       </c>
@@ -1032,6 +1134,9 @@
       </c>
       <c r="E14" t="s">
         <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>